<commit_message>
working with csv file type
</commit_message>
<xml_diff>
--- a/src/exportdata.xlsx
+++ b/src/exportdata.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -817,9 +817,78 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>62107f9c1a601c3edefd10d6</v>
+      </c>
+      <c r="B20" t="str">
+        <v>manjit nayak</v>
+      </c>
+      <c r="C20" t="str">
+        <v>manjit@gmail.com</v>
+      </c>
+      <c r="D20">
+        <v>87655566777</v>
+      </c>
+      <c r="E20" t="str">
+        <v>kolkata</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>6210b85eb1075b536f7fbc70</v>
+      </c>
+      <c r="B21" t="str">
+        <v>niyatee</v>
+      </c>
+      <c r="C21" t="str">
+        <v>gudi@gmail.com</v>
+      </c>
+      <c r="D21">
+        <v>1234567890</v>
+      </c>
+      <c r="E21" t="str">
+        <v>koraput</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>622734541f0216479f759b58</v>
+      </c>
+      <c r="B22" t="str">
+        <v>suraj</v>
+      </c>
+      <c r="C22" t="str">
+        <v>suraj@gmail.com</v>
+      </c>
+      <c r="D22">
+        <v>1123344444</v>
+      </c>
+      <c r="E22" t="str">
+        <v>pune</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>